<commit_message>
Bug de paginacion y eliminar producto de inventario
</commit_message>
<xml_diff>
--- a/backend/database/seeders/Catalogos/Productos.xlsx
+++ b/backend/database/seeders/Catalogos/Productos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="121">
   <si>
     <t>Desayunos y cenas</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Cereal con leche y fruta, incluye café</t>
   </si>
   <si>
-    <t>Asados a la Parilla</t>
-  </si>
-  <si>
     <t>Puyazo de 8 onz.</t>
   </si>
   <si>
@@ -309,6 +306,87 @@
   </si>
   <si>
     <t>Parrilla de 4 personas</t>
+  </si>
+  <si>
+    <t>Cimarrona Carlo</t>
+  </si>
+  <si>
+    <t>Cimarrona Virgen</t>
+  </si>
+  <si>
+    <t>Mineral con jugo de tomate preparado</t>
+  </si>
+  <si>
+    <t>Corona</t>
+  </si>
+  <si>
+    <t>Heineken</t>
+  </si>
+  <si>
+    <t>Guarniciones</t>
+  </si>
+  <si>
+    <t>Puré de papa</t>
+  </si>
+  <si>
+    <t>Papas Sazonadas</t>
+  </si>
+  <si>
+    <t>Papas Fritas</t>
+  </si>
+  <si>
+    <t>Frijoles de la Casa</t>
+  </si>
+  <si>
+    <t>Arroz</t>
+  </si>
+  <si>
+    <t>Ensalada Verde con Aderezo</t>
+  </si>
+  <si>
+    <t>Guacamole</t>
+  </si>
+  <si>
+    <t>Aperitivos</t>
+  </si>
+  <si>
+    <t>Mollejas Encebolladas con guacamole</t>
+  </si>
+  <si>
+    <t>Alitas de Pollo en Barbacoa</t>
+  </si>
+  <si>
+    <t>Con papas sazonadas</t>
+  </si>
+  <si>
+    <t>Alitas de Pollo Buffalo</t>
+  </si>
+  <si>
+    <t>Costillas al Horno en Barbacoa</t>
+  </si>
+  <si>
+    <t>Chorizo Argentino</t>
+  </si>
+  <si>
+    <t>1 lb de chorizo acompañado de guacamole, nachos y pico de gallo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fajitas de Puyazo </t>
+  </si>
+  <si>
+    <t>Asado y chorizo argentino</t>
+  </si>
+  <si>
+    <t>Nachos El Mirador</t>
+  </si>
+  <si>
+    <t>autoreferencia</t>
+  </si>
+  <si>
+    <t>promocion</t>
+  </si>
+  <si>
+    <t>Asados a la Parrilla</t>
   </si>
 </sst>
 </file>
@@ -636,35 +714,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="18.140625" customWidth="1"/>
+    <col min="2" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>76</v>
       </c>
-      <c r="G1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -674,11 +758,17 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -692,19 +782,25 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -718,19 +814,25 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>35</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -740,23 +842,29 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>35</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -769,20 +877,26 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>1</v>
+      <c r="E6" s="2">
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>35</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -796,19 +910,25 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
         <v>38</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -818,23 +938,29 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>45</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -848,19 +974,25 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>30</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -873,20 +1005,26 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10">
-        <v>1</v>
+      <c r="E10" s="2">
+        <v>9</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>35</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -896,23 +1034,29 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>35</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -926,61 +1070,79 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>25</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>13</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <v>85</v>
       </c>
-      <c r="H14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>12</v>
@@ -989,24 +1151,30 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
         <v>110</v>
       </c>
-      <c r="H15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>12</v>
@@ -1015,44 +1183,56 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17">
         <v>12</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>12</v>
@@ -1060,51 +1240,63 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18">
-        <v>1</v>
+      <c r="E18" s="2">
+        <v>17</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <v>90</v>
       </c>
-      <c r="H18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19">
         <v>12</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
         <v>125</v>
       </c>
-      <c r="H19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20">
         <v>12</v>
@@ -1113,61 +1305,79 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>300</v>
       </c>
-      <c r="H20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22">
         <v>20</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
         <v>120</v>
       </c>
-      <c r="H22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23">
         <v>20</v>
@@ -1176,24 +1386,30 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
         <v>100</v>
       </c>
-      <c r="H23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24">
         <v>20</v>
@@ -1202,47 +1418,59 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25">
         <v>20</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>24</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
         <v>90</v>
       </c>
-      <c r="H25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26">
         <v>20</v>
@@ -1251,21 +1479,27 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27">
         <v>20</v>
@@ -1274,47 +1508,59 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
         <v>100</v>
       </c>
-      <c r="H27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28">
         <v>20</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29">
         <v>20</v>
@@ -1322,25 +1568,31 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29">
-        <v>1</v>
+      <c r="E29" s="2">
+        <v>28</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
         <v>100</v>
       </c>
-      <c r="H29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30">
         <v>20</v>
@@ -1349,70 +1601,88 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31">
         <v>20</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32">
         <v>20</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
         <v>70</v>
       </c>
-      <c r="H32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33">
         <v>20</v>
@@ -1420,22 +1690,28 @@
       <c r="D33">
         <v>0</v>
       </c>
-      <c r="E33">
-        <v>1</v>
+      <c r="E33" s="2">
+        <v>32</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34">
         <v>20</v>
@@ -1443,56 +1719,74 @@
       <c r="D34">
         <v>0</v>
       </c>
-      <c r="E34">
-        <v>1</v>
+      <c r="E34" s="2">
+        <v>33</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35">
         <v>20</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37">
         <v>35</v>
@@ -1501,50 +1795,62 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
         <v>55</v>
       </c>
-      <c r="H37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38">
         <v>35</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2">
+        <v>37</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
         <v>50</v>
       </c>
-      <c r="H38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39">
         <v>35</v>
@@ -1553,24 +1859,30 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
         <v>45</v>
       </c>
-      <c r="H39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40">
         <v>35</v>
@@ -1579,61 +1891,79 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
         <v>50</v>
       </c>
-      <c r="H40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41">
         <v>35</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
         <v>50</v>
       </c>
-      <c r="H41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43">
         <v>41</v>
@@ -1642,55 +1972,73 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44">
         <v>41</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="2">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46">
         <v>44</v>
@@ -1699,50 +2047,62 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
         <v>50</v>
       </c>
-      <c r="H46" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47">
         <v>44</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="2">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
         <v>50</v>
       </c>
-      <c r="H47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C48">
         <v>44</v>
@@ -1751,61 +2111,79 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
         <v>70</v>
       </c>
-      <c r="H48" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50">
         <v>48</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="2">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
         <v>50</v>
       </c>
-      <c r="H50" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51">
         <v>48</v>
@@ -1814,24 +2192,30 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
         <v>50</v>
       </c>
-      <c r="H51" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C52">
         <v>48</v>
@@ -1840,35 +2224,47 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
         <v>45</v>
       </c>
-      <c r="H52" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D53" s="2">
+        <v>0</v>
+      </c>
+      <c r="E53" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54">
         <v>52</v>
@@ -1877,55 +2273,73 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55">
         <v>52</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55">
+        <v>54</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
         <v>2</v>
       </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-      <c r="G55">
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D56" s="2">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C57">
         <v>55</v>
@@ -1933,22 +2347,28 @@
       <c r="D57">
         <v>0</v>
       </c>
-      <c r="E57">
-        <v>1</v>
+      <c r="E57" s="2">
+        <v>56</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58">
         <v>55</v>
@@ -1956,45 +2376,57 @@
       <c r="D58">
         <v>0</v>
       </c>
-      <c r="E58">
-        <v>1</v>
+      <c r="E58" s="2">
+        <v>57</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C59">
         <v>55</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="2">
         <v>0</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C60">
         <v>55</v>
@@ -2003,127 +2435,772 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C62">
         <v>60</v>
       </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62">
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2">
+        <v>61</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
         <v>2</v>
       </c>
-      <c r="F62">
-        <v>1</v>
-      </c>
-      <c r="G62">
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C64">
         <v>62</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64">
+        <v>63</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="G64">
         <v>2</v>
       </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="G64">
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65">
         <v>62</v>
       </c>
-      <c r="D65">
-        <v>1</v>
+      <c r="D65" s="2">
+        <v>0</v>
       </c>
       <c r="E65">
+        <v>64</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65">
         <v>2</v>
       </c>
-      <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="G65">
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C66">
         <v>62</v>
       </c>
       <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2">
+        <v>65</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
         <v>2</v>
       </c>
-      <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="G66">
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
         <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67">
+        <v>62</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>66</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68">
+        <v>62</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>67</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>2</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>25</v>
+      </c>
+      <c r="J68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C69">
+        <v>62</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>68</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>2</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C70">
+        <v>62</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2">
+        <v>69</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72">
+        <v>70</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>71</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C73">
+        <v>70</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>72</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C74">
+        <v>70</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2">
+        <v>73</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75">
+        <v>70</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>74</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C76">
+        <v>70</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>75</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77">
+        <v>70</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>76</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C78">
+        <v>70</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2">
+        <v>77</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C79">
+        <v>70</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>78</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C81">
+        <v>79</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>80</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C82">
+        <v>79</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>81</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>45</v>
+      </c>
+      <c r="J82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C83">
+        <v>79</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>82</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>45</v>
+      </c>
+      <c r="J83" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C84">
+        <v>79</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2">
+        <v>83</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+      <c r="I84">
+        <v>50</v>
+      </c>
+      <c r="J84" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C85">
+        <v>79</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>84</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>75</v>
+      </c>
+      <c r="J85" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C86">
+        <v>79</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>85</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86">
+        <v>65</v>
+      </c>
+      <c r="J86" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C87">
+        <v>79</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>86</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en reservacion y ticket ...  logo incluido
</commit_message>
<xml_diff>
--- a/backend/database/seeders/Catalogos/Productos.xlsx
+++ b/backend/database/seeders/Catalogos/Productos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\restaurante-hotel\backend\database\seeders\Catalogos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hotel_restuarante\backend\database\seeders\Catalogos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -716,13 +716,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="8" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="141.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>